<commit_message>
Update Mining Profits Analysis.xlsx
change price
</commit_message>
<xml_diff>
--- a/Mining Profits Analysis.xlsx
+++ b/Mining Profits Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\GitHub\eth-gpu-mining-profitability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B3B44D-22F1-4011-B88A-FDA0CB6498A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AABFF8-31B5-44B6-90A9-E61CDEDA6266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{66B3F881-5B90-4DB1-B63B-2D100C44C995}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15375" xr2:uid="{66B3F881-5B90-4DB1-B63B-2D100C44C995}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Analysis" sheetId="3" r:id="rId1"/>
@@ -1127,24 +1127,6 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1166,12 +1148,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1490,7 +1490,7 @@
   <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,34 +1506,34 @@
   <sheetData>
     <row r="1" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:29" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
     </row>
     <row r="3" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="84">
         <v>44340</v>
       </c>
-      <c r="D3" s="90"/>
+      <c r="D3" s="84"/>
       <c r="U3"/>
       <c r="V3"/>
       <c r="W3"/>
@@ -1556,58 +1556,58 @@
       <c r="AC4"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="89"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="26">
         <f>'Electricity Calculations'!F6/100</f>
         <v>0.10324999999999999</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="89"/>
+      <c r="H5" s="83"/>
       <c r="I5" s="75">
         <v>3247</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="88" t="s">
+      <c r="K5" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="89"/>
+      <c r="L5" s="83"/>
       <c r="M5" s="76">
         <v>13.16</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="88" t="s">
+      <c r="A6" s="90"/>
+      <c r="B6" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="89"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="77">
         <v>613.84699999999998</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="88" t="s">
+      <c r="G6" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="89"/>
+      <c r="H6" s="83"/>
       <c r="I6" s="77">
         <v>2.2000000000000002</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="88" t="s">
+      <c r="K6" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="89"/>
+      <c r="L6" s="83"/>
       <c r="M6" s="81">
         <f>24*3600/$M$5*$I$6*$I$5/D6/1000000</f>
         <v>7.6401640690808459E-2</v>
@@ -1630,7 +1630,7 @@
       <c r="AC6"/>
     </row>
     <row r="7" spans="1:29" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
+      <c r="A7" s="90"/>
       <c r="U7"/>
       <c r="V7"/>
       <c r="W7"/>
@@ -1642,7 +1642,7 @@
       <c r="AC7"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="24" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="44" t="s">
         <v>52</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="33" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1810,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="47" t="s">
         <v>43</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
+      <c r="A12" s="90"/>
       <c r="B12" s="33" t="s">
         <v>15</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
+      <c r="A13" s="90"/>
       <c r="B13" s="47" t="s">
         <v>53</v>
       </c>
@@ -1993,7 +1993,7 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
+      <c r="A14" s="90"/>
       <c r="B14" s="33" t="s">
         <v>54</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>700</v>
       </c>
       <c r="E14" s="38">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="38">
         <v>450</v>
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
+      <c r="A15" s="90"/>
       <c r="B15" s="47" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
+      <c r="A16" s="90"/>
       <c r="B16" s="33" t="s">
         <v>20</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E16" s="58">
         <f t="shared" si="8"/>
-        <v>338.66245312196321</v>
+        <v>356.48679275996125</v>
       </c>
       <c r="F16" s="58">
         <f t="shared" ref="F16" si="9">F14/F13</f>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="17" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="25" t="s">
         <v>55</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="E17" s="55">
         <f t="shared" si="11"/>
-        <v>1.0777693146531122</v>
+        <v>1.0238808489204565</v>
       </c>
       <c r="F17" s="55">
         <f t="shared" ref="F17" si="12">F13*365/F14</f>
@@ -2242,25 +2242,25 @@
       </c>
     </row>
     <row r="18" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="92" t="s">
+      <c r="A18" s="90"/>
+      <c r="B18" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93"/>
-      <c r="M18" s="93"/>
-      <c r="N18" s="93"/>
-      <c r="O18" s="93"/>
-      <c r="P18" s="93"/>
-      <c r="Q18" s="94"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="88"/>
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
@@ -2272,50 +2272,50 @@
       <c r="AC18"/>
     </row>
     <row r="19" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="95" t="s">
+      <c r="A19" s="90"/>
+      <c r="B19" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="96"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="97"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="93"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="94"/>
     </row>
     <row r="20" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
-      <c r="B20" s="98" t="s">
+      <c r="A20" s="91"/>
+      <c r="B20" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="99"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="100"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="96"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="97"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="89" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="22" t="s">
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="83"/>
+      <c r="A23" s="90"/>
       <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
+      <c r="A24" s="90"/>
       <c r="B24" s="60" t="s">
         <v>42</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
+      <c r="A25" s="90"/>
       <c r="B25" s="40" t="s">
         <v>22</v>
       </c>
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
+      <c r="A26" s="90"/>
       <c r="B26" s="64" t="s">
         <v>20</v>
       </c>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="E26" s="66">
         <f t="shared" si="17"/>
-        <v>380.5977445712042</v>
+        <v>400.62920481179384</v>
       </c>
       <c r="F26" s="66">
         <f t="shared" ref="F26" si="18">IF(F25&gt;0,F$14/F25,"N/A")</f>
@@ -2591,7 +2591,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="83"/>
+      <c r="A27" s="90"/>
       <c r="B27" s="71" t="s">
         <v>21</v>
       </c>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="E27" s="73">
         <f t="shared" ref="E27:Q27" si="19">E25*365/E14</f>
-        <v>0.95901776930187221</v>
+        <v>0.91106688083677867</v>
       </c>
       <c r="F27" s="73">
         <f t="shared" ref="F27" si="20">F25*365/F14</f>
@@ -2657,29 +2657,29 @@
       </c>
     </row>
     <row r="28" spans="1:29" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
-      <c r="B28" s="85" t="s">
+      <c r="A28" s="91"/>
+      <c r="B28" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="86"/>
-      <c r="N28" s="86"/>
-      <c r="O28" s="86"/>
-      <c r="P28" s="86"/>
-      <c r="Q28" s="87"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
+      <c r="J28" s="99"/>
+      <c r="K28" s="99"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="99"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="100"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="89" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="22" t="s">
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="83"/>
+      <c r="A31" s="90"/>
       <c r="B31" s="4" t="s">
         <v>0</v>
       </c>
@@ -2757,7 +2757,7 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
+      <c r="A32" s="90"/>
       <c r="B32" s="60" t="s">
         <v>42</v>
       </c>
@@ -2823,7 +2823,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
+      <c r="A33" s="90"/>
       <c r="B33" s="40" t="s">
         <v>22</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
+      <c r="A34" s="90"/>
       <c r="B34" s="64" t="s">
         <v>20</v>
       </c>
@@ -2955,7 +2955,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="83"/>
+      <c r="A35" s="90"/>
       <c r="B35" s="71" t="s">
         <v>21</v>
       </c>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="E35" s="73">
         <f t="shared" si="27"/>
-        <v>-0.15133030990043228</v>
+        <v>-0.14376379440541068</v>
       </c>
       <c r="F35" s="73">
         <f t="shared" ref="F35" si="28">F33*365/F$14</f>
@@ -3021,29 +3021,29 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="84"/>
-      <c r="B36" s="85" t="s">
+      <c r="A36" s="91"/>
+      <c r="B36" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-      <c r="M36" s="86"/>
-      <c r="N36" s="86"/>
-      <c r="O36" s="86"/>
-      <c r="P36" s="86"/>
-      <c r="Q36" s="87"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="99"/>
+      <c r="L36" s="99"/>
+      <c r="M36" s="99"/>
+      <c r="N36" s="99"/>
+      <c r="O36" s="99"/>
+      <c r="P36" s="99"/>
+      <c r="Q36" s="100"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="89" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="22" t="s">
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
+      <c r="A39" s="90"/>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
@@ -3121,7 +3121,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
+      <c r="A40" s="90"/>
       <c r="B40" s="60" t="s">
         <v>42</v>
       </c>
@@ -3187,7 +3187,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
+      <c r="A41" s="90"/>
       <c r="B41" s="40" t="s">
         <v>22</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
+      <c r="A42" s="90"/>
       <c r="B42" s="64" t="s">
         <v>20</v>
       </c>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="E42" s="66">
         <f t="shared" ref="E42:F42" si="42">IF(E41&gt;0,E$14/E41,"N/A")</f>
-        <v>1641.038696972869</v>
+        <v>1727.4091547082833</v>
       </c>
       <c r="F42" s="66">
         <f t="shared" si="42"/>
@@ -3319,7 +3319,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="83"/>
+      <c r="A43" s="90"/>
       <c r="B43" s="71" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="E43" s="31">
         <f>E41*365/E$14</f>
-        <v>0.22242010543279375</v>
+        <v>0.21129910016115405</v>
       </c>
       <c r="F43" s="31">
         <f>F41*365/F$14</f>
@@ -3385,28 +3385,34 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="84"/>
-      <c r="B44" s="85" t="s">
+      <c r="A44" s="91"/>
+      <c r="B44" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="86"/>
-      <c r="D44" s="86"/>
-      <c r="E44" s="86"/>
-      <c r="F44" s="86"/>
-      <c r="G44" s="86"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="86"/>
-      <c r="J44" s="86"/>
-      <c r="K44" s="86"/>
-      <c r="L44" s="86"/>
-      <c r="M44" s="86"/>
-      <c r="N44" s="86"/>
-      <c r="O44" s="86"/>
-      <c r="P44" s="86"/>
-      <c r="Q44" s="87"/>
+      <c r="C44" s="99"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="99"/>
+      <c r="F44" s="99"/>
+      <c r="G44" s="99"/>
+      <c r="H44" s="99"/>
+      <c r="I44" s="99"/>
+      <c r="J44" s="99"/>
+      <c r="K44" s="99"/>
+      <c r="L44" s="99"/>
+      <c r="M44" s="99"/>
+      <c r="N44" s="99"/>
+      <c r="O44" s="99"/>
+      <c r="P44" s="99"/>
+      <c r="Q44" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="B44:Q44"/>
+    <mergeCell ref="B36:Q36"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B28:Q28"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="C3:D3"/>
@@ -3419,12 +3425,6 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="B44:Q44"/>
-    <mergeCell ref="B36:Q36"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B28:Q28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Update Mining Profits Analysis.xlsx"
This reverts commit 7394271678d93eb2269d33a86caee7d349d38dc3.
</commit_message>
<xml_diff>
--- a/Mining Profits Analysis.xlsx
+++ b/Mining Profits Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\GitHub\eth-gpu-mining-profitability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AABFF8-31B5-44B6-90A9-E61CDEDA6266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B3B44D-22F1-4011-B88A-FDA0CB6498A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15375" xr2:uid="{66B3F881-5B90-4DB1-B63B-2D100C44C995}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{66B3F881-5B90-4DB1-B63B-2D100C44C995}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Analysis" sheetId="3" r:id="rId1"/>
@@ -1127,6 +1127,24 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,30 +1166,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1490,7 +1490,7 @@
   <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,34 +1506,34 @@
   <sheetData>
     <row r="1" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:29" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
     </row>
     <row r="3" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="84">
+      <c r="C3" s="90">
         <v>44340</v>
       </c>
-      <c r="D3" s="84"/>
+      <c r="D3" s="90"/>
       <c r="U3"/>
       <c r="V3"/>
       <c r="W3"/>
@@ -1556,58 +1556,58 @@
       <c r="AC4"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="89"/>
       <c r="D5" s="26">
         <f>'Electricity Calculations'!F6/100</f>
         <v>0.10324999999999999</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="83"/>
+      <c r="H5" s="89"/>
       <c r="I5" s="75">
         <v>3247</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="83"/>
+      <c r="L5" s="89"/>
       <c r="M5" s="76">
         <v>13.16</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="90"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="83"/>
+      <c r="B6" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="83"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="77">
         <v>613.84699999999998</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="82" t="s">
+      <c r="G6" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="83"/>
+      <c r="H6" s="89"/>
       <c r="I6" s="77">
         <v>2.2000000000000002</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="83"/>
+      <c r="L6" s="89"/>
       <c r="M6" s="81">
         <f>24*3600/$M$5*$I$6*$I$5/D6/1000000</f>
         <v>7.6401640690808459E-2</v>
@@ -1630,7 +1630,7 @@
       <c r="AC6"/>
     </row>
     <row r="7" spans="1:29" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
+      <c r="A7" s="83"/>
       <c r="U7"/>
       <c r="V7"/>
       <c r="W7"/>
@@ -1642,7 +1642,7 @@
       <c r="AC7"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="24" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="90"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="44" t="s">
         <v>52</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="90"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="33" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1810,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="90"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="47" t="s">
         <v>43</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="33" t="s">
         <v>15</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="47" t="s">
         <v>53</v>
       </c>
@@ -1993,7 +1993,7 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="33" t="s">
         <v>54</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>700</v>
       </c>
       <c r="E14" s="38">
-        <v>1000</v>
+        <v>950</v>
       </c>
       <c r="F14" s="38">
         <v>450</v>
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="47" t="s">
         <v>19</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="33" t="s">
         <v>20</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E16" s="58">
         <f t="shared" si="8"/>
-        <v>356.48679275996125</v>
+        <v>338.66245312196321</v>
       </c>
       <c r="F16" s="58">
         <f t="shared" ref="F16" si="9">F14/F13</f>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="17" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="90"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="25" t="s">
         <v>55</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="E17" s="55">
         <f t="shared" si="11"/>
-        <v>1.0238808489204565</v>
+        <v>1.0777693146531122</v>
       </c>
       <c r="F17" s="55">
         <f t="shared" ref="F17" si="12">F13*365/F14</f>
@@ -2242,25 +2242,25 @@
       </c>
     </row>
     <row r="18" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="90"/>
-      <c r="B18" s="86" t="s">
+      <c r="A18" s="83"/>
+      <c r="B18" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="88"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="93"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="94"/>
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
@@ -2272,50 +2272,50 @@
       <c r="AC18"/>
     </row>
     <row r="19" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="92" t="s">
+      <c r="A19" s="83"/>
+      <c r="B19" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="93"/>
-      <c r="N19" s="93"/>
-      <c r="O19" s="93"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="94"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="96"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="96"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="97"/>
     </row>
     <row r="20" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="91"/>
-      <c r="B20" s="95" t="s">
+      <c r="A20" s="84"/>
+      <c r="B20" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="96"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="97"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="99"/>
+      <c r="N20" s="99"/>
+      <c r="O20" s="99"/>
+      <c r="P20" s="99"/>
+      <c r="Q20" s="100"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="82" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="22" t="s">
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="90"/>
+      <c r="A23" s="83"/>
       <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2393,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="90"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="60" t="s">
         <v>42</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="40" t="s">
         <v>22</v>
       </c>
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="90"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="64" t="s">
         <v>20</v>
       </c>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="E26" s="66">
         <f t="shared" si="17"/>
-        <v>400.62920481179384</v>
+        <v>380.5977445712042</v>
       </c>
       <c r="F26" s="66">
         <f t="shared" ref="F26" si="18">IF(F25&gt;0,F$14/F25,"N/A")</f>
@@ -2591,7 +2591,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="90"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="71" t="s">
         <v>21</v>
       </c>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="E27" s="73">
         <f t="shared" ref="E27:Q27" si="19">E25*365/E14</f>
-        <v>0.91106688083677867</v>
+        <v>0.95901776930187221</v>
       </c>
       <c r="F27" s="73">
         <f t="shared" ref="F27" si="20">F25*365/F14</f>
@@ -2657,29 +2657,29 @@
       </c>
     </row>
     <row r="28" spans="1:29" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="91"/>
-      <c r="B28" s="98" t="s">
+      <c r="A28" s="84"/>
+      <c r="B28" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="99"/>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
-      <c r="J28" s="99"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="99"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="100"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="87"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="82" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="22" t="s">
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="90"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="4" t="s">
         <v>0</v>
       </c>
@@ -2757,7 +2757,7 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A32" s="90"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="60" t="s">
         <v>42</v>
       </c>
@@ -2823,7 +2823,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="90"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="40" t="s">
         <v>22</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="90"/>
+      <c r="A34" s="83"/>
       <c r="B34" s="64" t="s">
         <v>20</v>
       </c>
@@ -2955,7 +2955,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="90"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="71" t="s">
         <v>21</v>
       </c>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="E35" s="73">
         <f t="shared" si="27"/>
-        <v>-0.14376379440541068</v>
+        <v>-0.15133030990043228</v>
       </c>
       <c r="F35" s="73">
         <f t="shared" ref="F35" si="28">F33*365/F$14</f>
@@ -3021,29 +3021,29 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="91"/>
-      <c r="B36" s="98" t="s">
+      <c r="A36" s="84"/>
+      <c r="B36" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="99"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="99"/>
-      <c r="Q36" s="100"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="86"/>
+      <c r="M36" s="86"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="86"/>
+      <c r="P36" s="86"/>
+      <c r="Q36" s="87"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="89" t="s">
+      <c r="A38" s="82" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="22" t="s">
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="90"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
@@ -3121,7 +3121,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="90"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="60" t="s">
         <v>42</v>
       </c>
@@ -3187,7 +3187,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="90"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="40" t="s">
         <v>22</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="64" t="s">
         <v>20</v>
       </c>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="E42" s="66">
         <f t="shared" ref="E42:F42" si="42">IF(E41&gt;0,E$14/E41,"N/A")</f>
-        <v>1727.4091547082833</v>
+        <v>1641.038696972869</v>
       </c>
       <c r="F42" s="66">
         <f t="shared" si="42"/>
@@ -3319,7 +3319,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="90"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="71" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="E43" s="31">
         <f>E41*365/E$14</f>
-        <v>0.21129910016115405</v>
+        <v>0.22242010543279375</v>
       </c>
       <c r="F43" s="31">
         <f>F41*365/F$14</f>
@@ -3385,34 +3385,28 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="91"/>
-      <c r="B44" s="98" t="s">
+      <c r="A44" s="84"/>
+      <c r="B44" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="99"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="99"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="99"/>
-      <c r="J44" s="99"/>
-      <c r="K44" s="99"/>
-      <c r="L44" s="99"/>
-      <c r="M44" s="99"/>
-      <c r="N44" s="99"/>
-      <c r="O44" s="99"/>
-      <c r="P44" s="99"/>
-      <c r="Q44" s="100"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="86"/>
+      <c r="K44" s="86"/>
+      <c r="L44" s="86"/>
+      <c r="M44" s="86"/>
+      <c r="N44" s="86"/>
+      <c r="O44" s="86"/>
+      <c r="P44" s="86"/>
+      <c r="Q44" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="B44:Q44"/>
-    <mergeCell ref="B36:Q36"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B28:Q28"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="C3:D3"/>
@@ -3425,6 +3419,12 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="B44:Q44"/>
+    <mergeCell ref="B36:Q36"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B28:Q28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="63" orientation="portrait" r:id="rId1"/>

</xml_diff>